<commit_message>
New version of NIS 2 german
Update the NIS 2 german version
</commit_message>
<xml_diff>
--- a/storage/app/repository/NIS2.de.xlsx
+++ b/storage/app/repository/NIS2.de.xlsx
@@ -684,7 +684,7 @@
       </c>
       <c r="F2" s="10" t="inlineStr">
         <is>
-          <t>Diese Richtlinie gilt für öffentliche oder private Einrichtungen der in Anhang I oder II genannten Art, die als mittlere Unternehmen gelten ... ihre Dienstleistungen erbringen oder ihre Tätigkeiten innerhalb der Union ausüben.
+          <t>Dieses Regelwerk richtet sich an besonders wichtige Einrichtungen und wichtige Einrichtungen im Sinne des BSI‑Gesetzes (BSIG) § 28 (Sektoren/Einrichtungsarten nach Anlagen 1 und 2) sowie – soweit einschlägig – an Einrichtungen der Bundesverwaltung (§ 29). Ob eine Organisation erfasst ist, ergibt sich aus Sektor, Einrichtungsart und ggf. Größen‑/Schwellenwerten.
 DE: BSIG §28 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
@@ -746,9 +746,8 @@
       </c>
       <c r="F3" s="10" t="inlineStr">
         <is>
-          <t>Mindestens die folgenden Informationen an die zuständigen Behörden übermitteln:
-- Name, Anschrift, Sektor, Liste der Mitgliedstaaten, in denen Dienstleistungen erbracht werden
-DE: BSIG §33, §59 (BGBl. I 2025 Nr. 301)</t>
+          <t>Besonders wichtige Einrichtungen, wichtige Einrichtungen sowie Domain‑Name‑Registry‑Diensteanbieter müssen sich spätestens drei Monate nach erstmaliger oder erneuter Einstufung beim BSI registrieren. Zu übermitteln sind u. a. Name (inkl. Rechtsform und ggf. Handelsregisternummer), Anschrift und aktuelle Kontaktdaten (inkl. E‑Mail‑Adresse, öffentliche IP‑Adressbereiche und Telefonnummern), relevanter Sektor/Branche, EU‑Mitgliedstaaten der Leistungserbringung sowie zuständige Aufsichtsbehörden. Änderungen sind fristgerecht zu melden.
+DE: BSIG §33 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
       <c r="G3" s="9" t="inlineStr">
@@ -810,7 +809,7 @@
       </c>
       <c r="F4" s="10" t="inlineStr">
         <is>
-          <t>Die Mitgliedstaaten stellen sicher, dass die Leitungsorgane wesentlicher und wichtiger Einrichtungen die von diesen Einrichtungen ergriffenen Cybersicherheits‑Risikomanagementmaßnahmen zur Erfüllung von Artikel 21 genehmigen, deren Umsetzung überwachen und für Verstöße der Einrichtungen gegen diesen Artikel haftbar gemacht werden können.
+          <t>Geschäftsleitungen besonders wichtiger Einrichtungen und wichtiger Einrichtungen sind verpflichtet, die nach BSIG § 30 erforderlichen Risikomanagementmaßnahmen umzusetzen und deren Umsetzung zu überwachen. Bei Pflichtverletzung können sie nach BSIG § 38 haftungsrechtlich in Anspruch genommen werden.
 DE: BSIG §38, §30 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
@@ -871,8 +870,8 @@
       </c>
       <c r="F5" s="10" t="inlineStr">
         <is>
-          <t>Die Mitgliedstaaten stellen sicher, dass die Mitglieder der Leitungsorgane wesentlicher und wichtiger Einrichtungen verpflichtet sind, regelmäßige Schulungen zu absolvieren ... Cybersicherheitspraktiken sowie deren Auswirkungen auf die von der Einrichtung erbrachten Dienstleistungen.
-DE: BSIG §38 (BGBl. I 2025 Nr. 301)</t>
+          <t>Die Geschäftsleitungen besonders wichtiger Einrichtungen und wichtiger Einrichtungen müssen regelmäßig an Schulungen teilnehmen, um ausreichende Kenntnisse und Fähigkeiten zur Erkennung und Bewertung von Risiken sowie von Risikomanagementpraktiken im Bereich der Sicherheit in der Informationstechnik zu erlangen und die Auswirkungen auf die von der Einrichtung erbrachten Dienste beurteilen zu können.
+DE: BSIG §38 Abs. 3 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
       <c r="G5" s="9" t="inlineStr">
@@ -934,8 +933,8 @@
       </c>
       <c r="F6" s="10" t="inlineStr">
         <is>
-          <t>Die Mitgliedstaaten stellen sicher, dass wesentliche und wichtige Einrichtungen geeignete und verhältnismäßige technische, operative ... und organisatorische Maßnahmen ergreifen ... und deren Schwere, einschließlich ihrer gesellschaftlichen und wirtschaftlichen Auswirkungen.
-DE: BSIG §30 (BGBl. I 2025 Nr. 301)</t>
+          <t>Es sind geeignete, verhältnismäßige und wirksame technische und organisatorische Maßnahmen zu ergreifen, um Störungen der Verfügbarkeit, Integrität und Vertraulichkeit der für die Erbringung der Dienste genutzten IT‑Systeme, Komponenten und Prozesse zu vermeiden und die Auswirkungen von Sicherheitsvorfällen möglichst gering zu halten. Die Maßnahmen sollen dem Stand der Technik entsprechen, einschlägige europäische und internationale Normen berücksichtigen und auf einem gefahrenübergreifenden Ansatz beruhen; die Einhaltung ist zu dokumentieren.
+DE: BSIG §30 Abs. 1–2 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
       <c r="G6" s="9" t="inlineStr">
@@ -999,8 +998,8 @@
       </c>
       <c r="F7" s="10" t="inlineStr">
         <is>
-          <t>Die Cybersicherheits‑Risikomanagementmaßnahmen sollten daher auch ... sowie anwendbare internationale Normen berücksichtigen, wie etwa die in der ISO/IEC‑27000‑Reihe enthaltenen.
-DE: BSIG §30 (BGBl. I 2025 Nr. 301)</t>
+          <t>Bei der Ausgestaltung der Risikomanagementmaßnahmen sollen einschlägige europäische und internationale Normen berücksichtigt werden. Als Orientierung können insbesondere ISO/IEC 27001 und die ISO/IEC‑27000‑Reihe (z. B. ISO/IEC 27002) herangezogen werden.
+DE: BSIG §30 Abs. 2 Satz 1 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
       <c r="G7" s="9" t="inlineStr">
@@ -1257,15 +1256,8 @@
       </c>
       <c r="F11" s="10" t="inlineStr">
         <is>
-          <t>Lieferkettensicherheit, einschließlich sicherheitsbezogener Aspekte der Beziehungen zwischen jeder Einrichtung und ihren direkten 
-Lieferanten oder Dienstleistern
-[...] Einrichtungen berücksichtigen die spezifischen Schwachstellen jedes direkten Lieferanten und Dienstleisters 
-und die Gesamtqualität der Produkte und der Cybersicherheitspraktiken ihrer Lieferanten und Dienstleister, einschließlich ihrer 
-sicheren Entwicklungsverfahren.
-Die Mitgliedstaaten stellen außerdem sicher, dass Einrichtungen bei der Prüfung, welche der in diesem Buchstaben genannten 
-Maßnahmen angemessen sind, verpflichtet sind, die Ergebnisse der koordinierten Sicherheitsrisikobewertungen kritischer Lieferketten 
-gemäß Artikel 22 Absatz 1 zu berücksichtigen.
-DE: BSIG §30 (BGBl. I 2025 Nr. 301)</t>
+          <t>Die Lieferkette ist abzusichern; hierzu gehören sicherheitsbezogene Aspekte der Beziehungen zu unmittelbaren Anbietern oder Diensteanbietern (z. B. Auswahlkriterien, vertragliche Mindestanforderungen, Überwachung sowie Incident‑Kommunikation).
+DE: BSIG §30 Abs. 2 Nr. 4 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
       <c r="G11" s="9" t="inlineStr">
@@ -1330,8 +1322,8 @@
       </c>
       <c r="F12" s="10" t="inlineStr">
         <is>
-          <t>Sicherheit bei Beschaffung, Entwicklung ... und Wartung von Netz‑ und Informationssystemen, einschließlich Umgang mit Schwachstellen und Offenlegung
-DE: BSIG §30 (BGBl. I 2025 Nr. 301)</t>
+          <t>Sicherheitsmaßnahmen bei Erwerb, Entwicklung und Wartung von informationstechnischen Systemen, Komponenten und Prozessen – einschließlich Management und Offenlegung von Schwachstellen – sind festzulegen und umzusetzen.
+DE: BSIG §30 Abs. 2 Nr. 5 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
       <c r="G12" s="9" t="inlineStr">
@@ -1455,8 +1447,8 @@
       </c>
       <c r="F14" s="10" t="inlineStr">
         <is>
-          <t>Grundlegende Cyberhygiene‑Praktiken und Cybersicherheits‑Schulungen
-DE: BSIG §30 (BGBl. I 2025 Nr. 301)</t>
+          <t>Grundlegende Schulungen und Sensibilisierungsmaßnahmen im Bereich der Sicherheit in der Informationstechnik sind durchzuführen und regelmäßig zu aktualisieren.
+DE: BSIG §30 Abs. 2 Nr. 7 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
       <c r="G14" s="9" t="inlineStr">
@@ -1976,8 +1968,8 @@
       </c>
       <c r="F22" s="10" t="inlineStr">
         <is>
-          <t>Um die Einhaltung bestimmter Anforderungen ... nach Artikel 21 nachzuweisen, können die Mitgliedstaaten wesentliche und wichtige Einrichtungen verpflichten, qualifizierte Vertrauensdienste zu nutzen
-DE: BSIG §30, §56 (BGBl. I 2025 Nr. 301)</t>
+          <t>Durch Rechtsverordnung kann festgelegt werden, dass bestimmte IKT‑Produkte, IKT‑Dienste oder IKT‑Prozesse nur verwendet werden dürfen, wenn sie über eine Cybersicherheitszertifizierung gemäß europäischen Schemata nach der Verordnung (EU) 2019/881 verfügen.
+DE: BSIG §30 Abs. 6, §56 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
       <c r="G22" s="9" t="inlineStr">
@@ -2036,16 +2028,7 @@
       </c>
       <c r="F23" s="10" t="inlineStr">
         <is>
-          <t>Die Mitgliedstaaten stellen sicher, dass die betroffenen Einrichtungen zum Zwecke der Meldung ... der CSIRT oder, soweit zutreffend, der zuständigen Behörde Folgendes übermitteln:
-(a) unverzüglich und in jedem Fall innerhalb von 24 Stunden nach ... Hinweise darauf, ob der erhebliche Sicherheitsvorfall vermutlich auf rechtswidrige oder böswillige Handlungen zurückzuführen ist oder grenzüberschreitende Auswirkungen haben könnte;
-(b) unverzüglich und in jedem Fall innerhalb von 72 Stunden nach ... eine Meldung des erheblichen Sicherheitsvorfalls, einschließlich – soweit verfügbar – einer ersten Bewertung des erheblichen Sicherheitsvorfalls, seiner Schwere und Auswirkungen, sowie – sofern verfügbar – der Indikatoren einer Kompromittierung;
-(c) auf Anforderung eines CSIRT oder, soweit zutreffend, der zuständigen Behörde, ... einen Zwischenbericht zu relevanten Status‑Updates;
-(d) einen Abschlussbericht spätestens einen Monat nach der Übermittlung ... der Sicherheitsvorfallmeldung nach Buchstabe (b), einschließlich:
-(i) einer detaillierten Beschreibung des Vorfalls, einschließlich seiner Schwere und Auswirkungen;
-(ii) der Art der Bedrohung oder Grundursache, die den Vorfall wahrscheinlich ausgelöst hat;
-(iii) angewandter und laufender Eindämmungsmaßnahmen;
-(iv) soweit zutreffend, der grenzüberschreitenden Auswirkungen des Vorfalls;
-(e) im Fall eines zum Zeitpunkt der Übermittlung ... laufenden Vorfalls ... den Abschlussbericht innerhalb eines Monats nach Abschluss der Bearbeitung des Vorfalls.
+          <t>Erhebliche Sicherheitsvorfälle sind über die gemeinsame Meldestelle zu melden: (1) frühe Erstmeldung spätestens binnen 24 Stunden nach Kenntniserlangung, (2) Meldung spätestens binnen 72 Stunden mit Bestätigung/Aktualisierung und erster Bewertung (inkl. Schweregrad/Auswirkungen und ggf. Kompromittierungsindikatoren), (3) auf Ersuchen Zwischenmeldungen, (4) Abschlussmeldung spätestens einen Monat nach der 72‑Stunden‑Meldung (bei andauerndem Vorfall zunächst Fortschrittsmeldung). Die Pflichten gelten frühestens ab Einrichtung des Meldewegs.
 DE: BSIG §32 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
@@ -2107,11 +2090,8 @@
       </c>
       <c r="F24" s="10" t="inlineStr">
         <is>
-          <t>Jeder Mitgliedstaat stellt sicher, dass wesentliche und wichtige Einrichtungen ihren CSIRT oder, soweit 
-zutreffend, ihre zuständige Behörde gemäß Absatz 4 unverzüglich über jeden Sicherheitsvorfall informieren, der erhebliche Auswirkungen auf die 
-Erbringung ihrer Dienstleistungen gemäß Absatz 3 hat (erheblicher Sicherheitsvorfall). Soweit angemessen, informieren die betroffenen Einrichtungen 
-unverzüglich die Empfänger ihrer Dienstleistungen über erhebliche Sicherheitsvorfälle, die die Erbringung dieser Dienstleistungen voraussichtlich nachteilig beeinträchtigen.
-DE: BSIG §32, §35, §59 (BGBl. I 2025 Nr. 301)</t>
+          <t>Im Fall eines erheblichen Sicherheitsvorfalls kann das BSI anordnen, dass Empfänger der Dienste unverzüglich über den Vorfall zu unterrichten sind, wenn die Erbringung des jeweiligen Dienstes beeinträchtigt sein könnte (ggf. auch per Veröffentlichung). Für bestimmte Sektoren bestehen zudem Pflichten, potenziell betroffene Empfänger über erhebliche Cyberbedrohungen sowie geeignete Abwehr‑ oder Abhilfemaßnahmen zu informieren.
+DE: BSIG §35 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
       <c r="G24" s="9" t="inlineStr">
@@ -2171,13 +2151,8 @@
       </c>
       <c r="F25" s="10" t="inlineStr">
         <is>
-          <t>Art. 32 (4) a) [wesentliche Einrichtungen]
-4. Die Mitgliedstaaten stellen sicher, dass ihre zuständigen Behörden, ... in Bezug auf wesentliche Einrichtungen mindestens befugt sind:
-(a) Warnungen über Verstöße der betroffenen Einrichtungen gegen diese Richtlinie auszusprechen; [...]
-Art. 33 (4) a) [wichtige Einrichtungen]
-4. Die Mitgliedstaaten stellen sicher, dass die zuständigen Behörden, ... in Bezug auf wichtige Einrichtungen mindestens befugt sind:
-(a) Warnungen über Verstöße der betroffenen Einrichtungen gegen diese Richtlinie auszusprechen; [...]
-DE: BSIG §13, §3 (BGBl. I 2025 Nr. 301)</t>
+          <t>Das BSI kann Warnungen und Informationen an die Öffentlichkeit oder an betroffene Kreise richten (z. B. zu Schwachstellen, Schadprogrammen, Datenverlust oder unbefugtem Datenzugriff sowie zu sicherheitsrelevanten IT‑Eigenschaften) und Sicherheitsmaßnahmen bzw. den Einsatz bestimmter Sicherheitsprodukte empfehlen. Hersteller betroffener Produkte sind grundsätzlich vorab zu informieren; Warnungen werden bei Wegfall der Voraussetzungen regelmäßig überprüft.
+DE: BSIG §13 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
       <c r="G25" s="9" t="inlineStr">
@@ -2237,20 +2212,8 @@
       </c>
       <c r="F26" s="10" t="inlineStr">
         <is>
-          <t>Art. 11 (3)
-3. Die CSIRTs haben insbesondere folgende Aufgaben:
-[...]
-(e)
-auf Antrag einer wesentlichen oder wichtigen Einrichtung, ... Schwachstellen mit potenziell erheblichen Auswirkungen zu erkennen; [...]
-Art. 32 (2) [wesentliche Einrichtungen]
-2. Die Mitgliedstaaten stellen sicher, dass die zuständigen Behörden, ... befugt sind, diese Einrichtungen mindestens folgenden Maßnahmen zu unterziehen:
-[...]
-(d) Sicherheitsscans auf der Grundlage objektiver, nichtdiskriminierender, fairer ... soweit dies mit der Mitwirkung der betroffenen Einrichtung erforderlich ist; [...]
-Art. 33 (2) [wichtige Einrichtungen]
-2. Die Mitgliedstaaten stellen sicher, dass die zuständigen Behörden, ... befugt sind, diese Einrichtungen mindestens folgenden Maßnahmen zu unterziehen:
-[...]
-(c) Sicherheitsscans auf der Grundlage objektiver, nichtdiskriminierender, fairer ... soweit dies mit der Mitwirkung der betroffenen Einrichtung erforderlich ist; [...]
-DE: BSIG §15, §3 (BGBl. I 2025 Nr. 301)</t>
+          <t>Das BSI kann Abfragen an den Schnittstellen öffentlich erreichbarer informationstechnischer Systeme zu öffentlichen Telekommunikationsnetzen durchführen, um bekannte Schwachstellen oder andere Sicherheitsrisiken zu detektieren – auch auf Ersuchen von Einrichtungen. Wird ein Risiko erkannt, informiert das BSI die Verantwortlichen unverzüglich und weist auf bestehende Möglichkeiten zur Abhilfe hin.
+DE: BSIG §15 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
       <c r="G26" s="9" t="inlineStr">
@@ -2314,7 +2277,7 @@
       </c>
       <c r="F27" s="10" t="inlineStr">
         <is>
-          <t>Die Mitgliedstaaten stellen sicher, dass Einrichtungen, die in den Anwendungsbereich ... fallen, und – soweit relevant – andere Einrichtungen ... Informationen austauschen, u. a. zu Cybersicherheits‑Risikomanagementmaßnahmen, Schwachstellen und Bedrohungen sowie zu Tools zur Erkennung von Cyberangriffen, sofern ein solcher Informationsaustausch:
+          <t>Das BSI betreibt eine Online‑Plattform zum Informationsaustausch mit wichtigen Einrichtungen, besonders wichtigen Einrichtungen und Einrichtungen der Bundesverwaltung. Der Austausch umfasst u. a. Cyberbedrohungen, Schwachstellen, Beinahevorfälle und IT‑Sicherheitsmaßnahmen; Hersteller, Lieferanten oder Dienstleister können einbezogen werden.
 DE: BSIG §6 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
@@ -2374,9 +2337,8 @@
       </c>
       <c r="F28" s="10" t="inlineStr">
         <is>
-          <t>Die Mitgliedstaaten stellen sicher, dass eine Einrichtung, die feststellt, dass sie die in Absatz 2 vorgesehenen Maßnahmen nicht einhält, 
-unverzüglich alle erforderlichen, angemessenen und verhältnismäßigen Korrekturmaßnahmen ergreift.
-DE: BSIG §62, §30, §32, §38, §61 (BGBl. I 2025 Nr. 301)</t>
+          <t>Rechtfertigen Tatsachen die Annahme, dass eine wichtige Einrichtung Verpflichtungen nach BSIG §30, §32 oder §38 nicht oder nicht richtig umsetzt, kann das BSI die Einhaltung überprüfen und Aufsichts‑/Durchsetzungsmaßnahmen ergreifen (Maßnahmen nach §61). Gegenüber besonders wichtigen Einrichtungen kann das BSI u. a. Audits/Prüfungen/Zertifizierungen anordnen, Nachweise verlangen und bei Mängeln konkrete Abhilfemaßnahmen sowie Mängelbeseitigungspläne anordnen.
+DE: BSIG §62 i. V. m. §61 (BGBl. I 2025 Nr. 301)</t>
         </is>
       </c>
       <c r="G28" s="9" t="inlineStr">

</xml_diff>